<commit_message>
Remove the forgotten data from the spreadsheet
</commit_message>
<xml_diff>
--- a/sheet/model.xlsx
+++ b/sheet/model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadrian\Downloads\teste\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6123C6-00B2-4A18-B632-203E58797525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F76F63-B5ED-4D87-B7CF-508657DC98FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle Aditivos" sheetId="1" r:id="rId1"/>
@@ -468,6 +468,12 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -542,12 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -768,7 +768,7 @@
   <dimension ref="A1:AA953"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -805,19 +805,19 @@
       <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+      <c r="A2" s="30">
         <f ca="1">NOW()</f>
-        <v>46036.142601273146</v>
+        <v>46036.626430902776</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="5"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
@@ -828,14 +828,14 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
       <c r="I3" s="5"/>
       <c r="J3" s="4"/>
       <c r="K3" s="5"/>
@@ -914,11 +914,9 @@
     </row>
     <row r="6" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="11"/>
-      <c r="D6" s="44">
-        <v>47027</v>
-      </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="1"/>
@@ -943,9 +941,9 @@
     </row>
     <row r="7" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="11"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="1"/>
@@ -970,9 +968,9 @@
     </row>
     <row r="8" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="11"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="1"/>
@@ -997,9 +995,9 @@
     </row>
     <row r="9" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="11"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="1"/>
@@ -1024,9 +1022,9 @@
     </row>
     <row r="10" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="11"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="1"/>
@@ -1266,10 +1264,10 @@
       <c r="AA18" s="1"/>
     </row>
     <row r="19" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="33"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="6">
         <f>SUM(E6:E18)</f>
         <v>0</v>
@@ -1305,20 +1303,20 @@
       <c r="AA19" s="1"/>
     </row>
     <row r="20" spans="1:27" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="34">
+      <c r="D20" s="33"/>
+      <c r="E20" s="36">
         <f>E19+F19</f>
         <v>0</v>
       </c>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36">
+      <c r="F20" s="37"/>
+      <c r="G20" s="38">
         <f>G19+H19</f>
         <v>0</v>
       </c>
-      <c r="H20" s="37"/>
+      <c r="H20" s="39"/>
       <c r="I20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1392,16 +1390,16 @@
       <c r="AA22" s="1"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="23"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1423,14 +1421,14 @@
       <c r="AA23" s="1"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1452,14 +1450,14 @@
       <c r="AA24" s="1"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>

</xml_diff>